<commit_message>
Goryachy Klyuch (18-23, without saldo)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>saldo</t>
+  </si>
+  <si>
+    <t>Горячий ключ МР</t>
   </si>
   <si>
     <t>Горячий ключ</t>
@@ -118,7 +121,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -135,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -147,6 +150,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -429,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U12"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
@@ -586,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="2">
-        <f t="shared" ref="B4:B12" si="0">B3+1</f>
+        <f t="shared" ref="B4:B9" si="0">B3+1</f>
         <v>2012</v>
       </c>
       <c r="C4" s="2">
@@ -734,7 +740,9 @@
         <v>9796</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2">
+        <v>26828</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="3">
@@ -769,125 +777,236 @@
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="4">
         <f t="shared" si="0"/>
         <v>2016</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="4">
         <v>63.61</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>9596</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="4">
         <v>515</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>28700</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="3">
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="5">
         <f>154/(C8/10)</f>
         <v>24.210029869517374</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="5">
         <f>284/(C8/10)</f>
         <v>44.647068071058008</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="5">
         <f>1215/(C8/10)</f>
         <v>191.00770319132212</v>
       </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4">
         <v>3294</v>
       </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2">
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4">
+        <v>149.4</v>
+      </c>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4">
         <v>29655</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="4">
         <v>390</v>
       </c>
-      <c r="U8" s="2">
+      <c r="U8" s="4">
         <v>1490</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="4">
         <f t="shared" si="0"/>
         <v>2017</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="4">
         <v>65.099999999999994</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>8896</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="4">
         <v>510</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>29940</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="3">
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="5">
         <v>18.899999999999999</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="4">
         <v>34.700000000000003</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="5">
         <f>1099/(C9/10)</f>
         <v>168.81720430107526</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="4">
         <v>1737.7</v>
       </c>
-      <c r="M9" s="2"/>
+      <c r="M9" s="4"/>
       <c r="N9" s="4">
         <v>2377</v>
       </c>
-      <c r="O9" s="2">
+      <c r="O9" s="4">
         <v>3389</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="4">
         <v>471</v>
       </c>
-      <c r="Q9" s="2">
+      <c r="Q9" s="4">
         <v>80.5</v>
       </c>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2">
+      <c r="R9" s="4"/>
+      <c r="S9" s="4">
         <v>34319</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="4">
         <v>429</v>
       </c>
-      <c r="U9" s="2">
+      <c r="U9" s="4">
         <v>1028</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C10" s="2">
+        <v>37.475000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <v>31404</v>
+      </c>
+      <c r="O10" s="2">
+        <v>3495.3</v>
+      </c>
+      <c r="P10" s="2">
+        <v>94.3</v>
+      </c>
+      <c r="S10" s="2">
+        <v>46980</v>
+      </c>
+      <c r="T10" s="2">
+        <v>22.9</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C11" s="2">
+        <v>38.972000000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <v>34491</v>
+      </c>
+      <c r="O11" s="2">
+        <v>2533.6999999999998</v>
+      </c>
+      <c r="S11" s="2">
+        <v>46733.5</v>
+      </c>
+      <c r="T11" s="2">
+        <v>22.4</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C12" s="2">
+        <v>40.298999999999999</v>
+      </c>
+      <c r="F12" s="2">
+        <v>38996</v>
+      </c>
+      <c r="O12" s="2">
+        <v>2392.9</v>
+      </c>
+      <c r="S12" s="2">
+        <v>50203.3</v>
+      </c>
+      <c r="T12" s="2">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C13" s="2">
+        <v>40.902999999999999</v>
+      </c>
+      <c r="F13" s="2">
+        <v>35126.300000000003</v>
+      </c>
+      <c r="O13" s="2">
+        <v>2665.5</v>
+      </c>
+      <c r="S13" s="2">
+        <v>26942.7</v>
+      </c>
+      <c r="T13" s="2">
+        <v>91.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C14" s="2">
+        <v>41.481999999999999</v>
+      </c>
+      <c r="F14" s="2">
+        <v>42049</v>
+      </c>
+      <c r="O14" s="2">
+        <v>4270.8999999999996</v>
+      </c>
+      <c r="S14" s="2">
+        <v>14680.8</v>
+      </c>
+      <c r="T14" s="2">
+        <v>210.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Anapa and Gelendzhik 2023 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>Горячий ключ</t>
+  </si>
+  <si>
+    <t>Анапа</t>
+  </si>
+  <si>
+    <t>Геленджик</t>
   </si>
 </sst>
 </file>
@@ -435,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +605,7 @@
         <v>58.33</v>
       </c>
       <c r="D4" s="2">
-        <v>9259</v>
+        <v>9.2590000000000003</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -639,7 +645,7 @@
         <v>59.3</v>
       </c>
       <c r="D5" s="2">
-        <v>9375</v>
+        <v>9.375</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -688,7 +694,7 @@
         <v>60.44</v>
       </c>
       <c r="D6" s="2">
-        <v>9863</v>
+        <v>9.8629999999999995</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -737,7 +743,7 @@
         <v>61.9</v>
       </c>
       <c r="D7" s="2">
-        <v>9796</v>
+        <v>9.7959999999999994</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2">
@@ -788,7 +794,7 @@
         <v>63.61</v>
       </c>
       <c r="D8" s="4">
-        <v>9596</v>
+        <v>9.5960000000000001</v>
       </c>
       <c r="E8" s="4">
         <v>515</v>
@@ -843,7 +849,7 @@
         <v>65.099999999999994</v>
       </c>
       <c r="D9" s="4">
-        <v>8896</v>
+        <v>8.8960000000000008</v>
       </c>
       <c r="E9" s="4">
         <v>510</v>
@@ -990,22 +996,196 @@
         <v>22</v>
       </c>
       <c r="B14" s="2">
+        <v>2022</v>
+      </c>
+      <c r="U14" s="2">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="2">
         <v>2023</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C15" s="2">
         <v>41.481999999999999</v>
       </c>
-      <c r="F14" s="2">
+      <c r="D15" s="2">
+        <v>7.6509999999999998</v>
+      </c>
+      <c r="E15" s="2">
+        <v>162</v>
+      </c>
+      <c r="F15" s="2">
         <v>42049</v>
       </c>
-      <c r="O14" s="2">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
+        <v>885</v>
+      </c>
+      <c r="O15" s="2">
         <v>4270.8999999999996</v>
       </c>
-      <c r="S14" s="2">
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2">
+        <v>95.557000000000002</v>
+      </c>
+      <c r="R15" s="2">
+        <v>1198</v>
+      </c>
+      <c r="S15" s="2">
         <v>14680.8</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T15" s="2">
         <v>210.2</v>
+      </c>
+      <c r="U15" s="2">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D18" s="2">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="E18" s="2">
+        <v>643</v>
+      </c>
+      <c r="F18" s="2">
+        <v>49270</v>
+      </c>
+      <c r="N18" s="2">
+        <v>3373</v>
+      </c>
+      <c r="O18" s="2">
+        <v>5465.4</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>592.06500000000005</v>
+      </c>
+      <c r="R18" s="2">
+        <v>7363</v>
+      </c>
+      <c r="S18" s="2">
+        <v>49034.2</v>
+      </c>
+      <c r="T18" s="2">
+        <v>3455.4180000000001</v>
+      </c>
+      <c r="U18" s="2">
+        <v>4899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2023</v>
+      </c>
+      <c r="D19" s="2">
+        <v>19.093</v>
+      </c>
+      <c r="E19" s="2">
+        <v>96</v>
+      </c>
+      <c r="F19" s="2">
+        <v>56182</v>
+      </c>
+      <c r="N19" s="2">
+        <v>2396</v>
+      </c>
+      <c r="O19" s="2">
+        <v>3456.8</v>
+      </c>
+      <c r="P19" s="2">
+        <v>12221.3</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>114.619</v>
+      </c>
+      <c r="R19" s="2">
+        <v>646</v>
+      </c>
+      <c r="S19" s="2">
+        <v>32472.3</v>
+      </c>
+      <c r="T19" s="2">
+        <v>1040.3309999999999</v>
+      </c>
+      <c r="U19" s="2">
+        <v>407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GK, Anapa, Gelend. 2022 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U19"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,6 +990,9 @@
       <c r="T13" s="2">
         <v>91.8</v>
       </c>
+      <c r="U13" s="2">
+        <v>1529</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -997,6 +1000,36 @@
       </c>
       <c r="B14" s="2">
         <v>2022</v>
+      </c>
+      <c r="D14" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>225</v>
+      </c>
+      <c r="F14" s="2">
+        <v>38166</v>
+      </c>
+      <c r="N14" s="2">
+        <v>873</v>
+      </c>
+      <c r="O14" s="2">
+        <v>3265.1</v>
+      </c>
+      <c r="P14" s="2">
+        <v>213.9</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>85.277000000000001</v>
+      </c>
+      <c r="R14" s="2">
+        <v>991</v>
+      </c>
+      <c r="S14" s="2">
+        <v>15205.4</v>
+      </c>
+      <c r="T14" s="2">
+        <v>466.7</v>
       </c>
       <c r="U14" s="2">
         <v>1148</v>
@@ -1056,28 +1089,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2">
-        <v>704</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1085,28 +1097,7 @@
         <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="2"/>
-      <c r="U17" s="2">
-        <v>-366</v>
+        <v>2021</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1114,37 +1105,50 @@
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>2023</v>
+        <v>2022</v>
+      </c>
+      <c r="C18" s="2">
+        <v>81.863</v>
       </c>
       <c r="D18" s="2">
-        <v>30.728999999999999</v>
+        <v>29</v>
       </c>
       <c r="E18" s="2">
-        <v>643</v>
+        <v>929</v>
       </c>
       <c r="F18" s="2">
-        <v>49270</v>
-      </c>
+        <v>42361</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
       <c r="N18" s="2">
-        <v>3373</v>
+        <v>3334</v>
       </c>
       <c r="O18" s="2">
-        <v>5465.4</v>
+        <v>3321.5</v>
+      </c>
+      <c r="P18" s="2">
+        <v>150.80000000000001</v>
       </c>
       <c r="Q18" s="2">
-        <v>592.06500000000005</v>
+        <v>532.51300000000003</v>
       </c>
       <c r="R18" s="2">
-        <v>7363</v>
+        <v>5456</v>
       </c>
       <c r="S18" s="2">
-        <v>49034.2</v>
+        <v>41571.199999999997</v>
       </c>
       <c r="T18" s="2">
-        <v>3455.4180000000001</v>
+        <v>2116</v>
       </c>
       <c r="U18" s="2">
-        <v>4899</v>
+        <v>704</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1152,39 +1156,134 @@
         <v>24</v>
       </c>
       <c r="B19" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C19" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D19" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E19" s="2">
+        <v>212</v>
+      </c>
+      <c r="F19" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O19" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P19" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q19" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R19" s="2">
+        <v>970</v>
+      </c>
+      <c r="S19" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T19" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U19" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
         <v>2023</v>
       </c>
-      <c r="D19" s="2">
+      <c r="C20" s="2">
+        <v>82.691999999999993</v>
+      </c>
+      <c r="D20" s="2">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="E20" s="2">
+        <v>643</v>
+      </c>
+      <c r="F20" s="2">
+        <v>49270</v>
+      </c>
+      <c r="N20" s="2">
+        <v>3373</v>
+      </c>
+      <c r="O20" s="2">
+        <v>5465.4</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>592.06500000000005</v>
+      </c>
+      <c r="R20" s="2">
+        <v>7363</v>
+      </c>
+      <c r="S20" s="2">
+        <v>49034.2</v>
+      </c>
+      <c r="T20" s="2">
+        <v>3455.4180000000001</v>
+      </c>
+      <c r="U20" s="2">
+        <v>4899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C21" s="2">
+        <v>80.296000000000006</v>
+      </c>
+      <c r="D21" s="2">
         <v>19.093</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E21" s="2">
         <v>96</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F21" s="2">
         <v>56182</v>
       </c>
-      <c r="N19" s="2">
+      <c r="N21" s="2">
         <v>2396</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O21" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P21" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q21" s="2">
         <v>114.619</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R21" s="2">
         <v>646</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S21" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T21" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U21" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Beforeschool, invest for 2022-2021
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -444,7 +444,7 @@
   <dimension ref="A1:U21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,6 +981,9 @@
       <c r="F13" s="2">
         <v>35126.300000000003</v>
       </c>
+      <c r="L13">
+        <v>1384.127</v>
+      </c>
       <c r="O13" s="2">
         <v>2665.5</v>
       </c>
@@ -1010,6 +1013,12 @@
       <c r="F14" s="2">
         <v>38166</v>
       </c>
+      <c r="H14" s="2">
+        <v>2544</v>
+      </c>
+      <c r="L14">
+        <v>863.57799999999997</v>
+      </c>
       <c r="N14" s="2">
         <v>873</v>
       </c>
@@ -1055,7 +1064,9 @@
         <v>42049</v>
       </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>2139</v>
+      </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -1091,6 +1102,9 @@
       <c r="B16" s="2">
         <v>2021</v>
       </c>
+      <c r="L16">
+        <v>15703.486000000001</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
@@ -1099,6 +1113,9 @@
       <c r="B17" s="2">
         <v>2021</v>
       </c>
+      <c r="L17">
+        <v>10326.647999999999</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
@@ -1120,11 +1137,15 @@
         <v>42361</v>
       </c>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>8508</v>
+      </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="L18" s="2">
+        <v>26447.994999999999</v>
+      </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2">
         <v>3334</v>
@@ -1171,11 +1192,15 @@
         <v>48384</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>5843</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="L19" s="2">
+        <v>7713.7349999999997</v>
+      </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2">
         <v>2489</v>
@@ -1221,6 +1246,9 @@
       <c r="F20" s="2">
         <v>49270</v>
       </c>
+      <c r="H20" s="2">
+        <v>8508</v>
+      </c>
       <c r="N20" s="2">
         <v>3373</v>
       </c>
@@ -1261,6 +1289,9 @@
       </c>
       <c r="F21" s="2">
         <v>56182</v>
+      </c>
+      <c r="H21" s="2">
+        <v>5703</v>
       </c>
       <c r="N21" s="2">
         <v>2396</v>

</xml_diff>

<commit_message>
Anapa, Gelen, GK 2021 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,6 +967,9 @@
       <c r="T12" s="2">
         <v>61.8</v>
       </c>
+      <c r="U12" s="2">
+        <v>2003</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -978,14 +981,32 @@
       <c r="C13" s="2">
         <v>40.902999999999999</v>
       </c>
+      <c r="D13" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E13" s="2">
+        <v>274</v>
+      </c>
       <c r="F13" s="2">
         <v>35126.300000000003</v>
       </c>
       <c r="L13">
         <v>1384.127</v>
       </c>
+      <c r="N13" s="2">
+        <v>850</v>
+      </c>
       <c r="O13" s="2">
         <v>2665.5</v>
+      </c>
+      <c r="P13" s="2">
+        <v>151.80000000000001</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>76.257999999999996</v>
+      </c>
+      <c r="R13" s="2">
+        <v>1089</v>
       </c>
       <c r="S13" s="2">
         <v>26942.7</v>
@@ -1003,6 +1024,9 @@
       </c>
       <c r="B14" s="2">
         <v>2022</v>
+      </c>
+      <c r="C14" s="2">
+        <v>41</v>
       </c>
       <c r="D14" s="2">
         <v>8.5</v>
@@ -1100,10 +1124,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>2021</v>
-      </c>
-      <c r="L16">
-        <v>15703.486000000001</v>
+        <v>2020</v>
+      </c>
+      <c r="C16" s="2">
+        <v>88.879000000000005</v>
+      </c>
+      <c r="U16" s="2">
+        <v>7130</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1111,10 +1138,13 @@
         <v>24</v>
       </c>
       <c r="B17" s="2">
-        <v>2021</v>
-      </c>
-      <c r="L17">
-        <v>10326.647999999999</v>
+        <v>2020</v>
+      </c>
+      <c r="C17" s="2">
+        <v>76.783000000000001</v>
+      </c>
+      <c r="U17" s="2">
+        <v>-1278</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1122,54 +1152,46 @@
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C18" s="2">
         <v>81.863</v>
       </c>
       <c r="D18" s="2">
-        <v>29</v>
+        <v>28.3</v>
       </c>
       <c r="E18" s="2">
-        <v>929</v>
+        <v>1017</v>
       </c>
       <c r="F18" s="2">
-        <v>42361</v>
-      </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2">
-        <v>8508</v>
-      </c>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2">
-        <v>26447.994999999999</v>
-      </c>
-      <c r="M18" s="2"/>
+        <v>38808</v>
+      </c>
+      <c r="L18">
+        <v>15703.486000000001</v>
+      </c>
       <c r="N18" s="2">
-        <v>3334</v>
+        <v>3561</v>
       </c>
       <c r="O18" s="2">
-        <v>3321.5</v>
+        <v>2466.6999999999998</v>
       </c>
       <c r="P18" s="2">
-        <v>150.80000000000001</v>
+        <v>289.2</v>
       </c>
       <c r="Q18" s="2">
-        <v>532.51300000000003</v>
+        <v>523.16399999999999</v>
       </c>
       <c r="R18" s="2">
-        <v>5456</v>
+        <v>8415</v>
       </c>
       <c r="S18" s="2">
-        <v>41571.199999999997</v>
+        <v>36829.599999999999</v>
       </c>
       <c r="T18" s="2">
-        <v>2116</v>
+        <v>1014.6</v>
       </c>
       <c r="U18" s="2">
-        <v>704</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1177,54 +1199,46 @@
         <v>24</v>
       </c>
       <c r="B19" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C19" s="2">
         <v>80.203999999999994</v>
       </c>
       <c r="D19" s="2">
-        <v>18.2</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E19" s="2">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="F19" s="2">
-        <v>48384</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2">
-        <v>5843</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2">
-        <v>7713.7349999999997</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>42904</v>
+      </c>
+      <c r="L19">
+        <v>10326.647999999999</v>
+      </c>
       <c r="N19" s="2">
-        <v>2489</v>
+        <v>2565</v>
       </c>
       <c r="O19" s="2">
-        <v>2937.3</v>
+        <v>1318.4</v>
       </c>
       <c r="P19" s="2">
-        <v>3009</v>
+        <v>4092.5</v>
       </c>
       <c r="Q19" s="2">
-        <v>188.37</v>
+        <v>101.312</v>
       </c>
       <c r="R19" s="2">
-        <v>970</v>
+        <v>552</v>
       </c>
       <c r="S19" s="2">
-        <v>27967.1</v>
+        <v>24283.1</v>
       </c>
       <c r="T19" s="2">
-        <v>631.20000000000005</v>
+        <v>992.7</v>
       </c>
       <c r="U19" s="2">
-        <v>-366</v>
+        <v>-258</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1232,43 +1246,54 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C20" s="2">
-        <v>82.691999999999993</v>
+        <v>81.863</v>
       </c>
       <c r="D20" s="2">
-        <v>30.728999999999999</v>
+        <v>29</v>
       </c>
       <c r="E20" s="2">
-        <v>643</v>
+        <v>929</v>
       </c>
       <c r="F20" s="2">
-        <v>49270</v>
-      </c>
+        <v>42361</v>
+      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2">
         <v>8508</v>
       </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2">
+        <v>26447.994999999999</v>
+      </c>
+      <c r="M20" s="2"/>
       <c r="N20" s="2">
-        <v>3373</v>
+        <v>3334</v>
       </c>
       <c r="O20" s="2">
-        <v>5465.4</v>
+        <v>3321.5</v>
+      </c>
+      <c r="P20" s="2">
+        <v>150.80000000000001</v>
       </c>
       <c r="Q20" s="2">
-        <v>592.06500000000005</v>
+        <v>532.51300000000003</v>
       </c>
       <c r="R20" s="2">
-        <v>7363</v>
+        <v>5456</v>
       </c>
       <c r="S20" s="2">
-        <v>49034.2</v>
+        <v>41571.199999999997</v>
       </c>
       <c r="T20" s="2">
-        <v>3455.4180000000001</v>
+        <v>2116</v>
       </c>
       <c r="U20" s="2">
-        <v>4899</v>
+        <v>704</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -1276,45 +1301,144 @@
         <v>24</v>
       </c>
       <c r="B21" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C21" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D21" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E21" s="2">
+        <v>212</v>
+      </c>
+      <c r="F21" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2">
+        <v>5843</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2">
+        <v>7713.7349999999997</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O21" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P21" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R21" s="2">
+        <v>970</v>
+      </c>
+      <c r="S21" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T21" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U21" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="2">
         <v>2023</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C22" s="2">
+        <v>82.691999999999993</v>
+      </c>
+      <c r="D22" s="2">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>643</v>
+      </c>
+      <c r="F22" s="2">
+        <v>49270</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8508</v>
+      </c>
+      <c r="N22" s="2">
+        <v>3373</v>
+      </c>
+      <c r="O22" s="2">
+        <v>5465.4</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>592.06500000000005</v>
+      </c>
+      <c r="R22" s="2">
+        <v>7363</v>
+      </c>
+      <c r="S22" s="2">
+        <v>49034.2</v>
+      </c>
+      <c r="T22" s="2">
+        <v>3455.4180000000001</v>
+      </c>
+      <c r="U22" s="2">
+        <v>4899</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C23" s="2">
         <v>80.296000000000006</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D23" s="2">
         <v>19.093</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E23" s="2">
         <v>96</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F23" s="2">
         <v>56182</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H23" s="2">
         <v>5703</v>
       </c>
-      <c r="N21" s="2">
+      <c r="N23" s="2">
         <v>2396</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O23" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P23" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q23" s="2">
         <v>114.619</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R23" s="2">
         <v>646</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S23" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T23" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U23" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Anapa, GK and Gelen. 2020 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U23"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -955,11 +955,29 @@
       <c r="C12" s="2">
         <v>40.298999999999999</v>
       </c>
+      <c r="D12" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="E12" s="2">
+        <v>799</v>
+      </c>
       <c r="F12" s="2">
         <v>38996</v>
       </c>
+      <c r="N12" s="2">
+        <v>880</v>
+      </c>
       <c r="O12" s="2">
         <v>2392.9</v>
+      </c>
+      <c r="P12" s="2">
+        <v>117.2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>66.64</v>
+      </c>
+      <c r="R12" s="2">
+        <v>990</v>
       </c>
       <c r="S12" s="2">
         <v>50203.3</v>
@@ -1119,32 +1137,48 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C16" s="2">
-        <v>88.879000000000005</v>
-      </c>
-      <c r="U16" s="2">
-        <v>7130</v>
-      </c>
-    </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="2">
         <v>2020</v>
       </c>
       <c r="C17" s="2">
-        <v>76.783000000000001</v>
+        <v>88.879000000000005</v>
+      </c>
+      <c r="D17" s="2">
+        <v>26.6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5378</v>
+      </c>
+      <c r="F17" s="2">
+        <v>34049</v>
+      </c>
+      <c r="N17" s="2">
+        <v>3562</v>
+      </c>
+      <c r="O17" s="2">
+        <v>1845</v>
+      </c>
+      <c r="P17" s="2">
+        <v>637.29999999999995</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>526.50900000000001</v>
+      </c>
+      <c r="R17" s="2">
+        <v>9241</v>
+      </c>
+      <c r="S17" s="2">
+        <v>26593</v>
+      </c>
+      <c r="T17" s="2">
+        <v>753.2</v>
       </c>
       <c r="U17" s="2">
-        <v>-1278</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1196,49 +1230,57 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C19" s="2">
-        <v>80.203999999999994</v>
+        <v>81.863</v>
       </c>
       <c r="D19" s="2">
-        <v>18.600000000000001</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2">
-        <v>262</v>
+        <v>929</v>
       </c>
       <c r="F19" s="2">
-        <v>42904</v>
-      </c>
-      <c r="L19">
-        <v>10326.647999999999</v>
-      </c>
+        <v>42361</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2">
+        <v>8508</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2">
+        <v>26447.994999999999</v>
+      </c>
+      <c r="M19" s="2"/>
       <c r="N19" s="2">
-        <v>2565</v>
+        <v>3334</v>
       </c>
       <c r="O19" s="2">
-        <v>1318.4</v>
+        <v>3321.5</v>
       </c>
       <c r="P19" s="2">
-        <v>4092.5</v>
+        <v>150.80000000000001</v>
       </c>
       <c r="Q19" s="2">
-        <v>101.312</v>
+        <v>532.51300000000003</v>
       </c>
       <c r="R19" s="2">
-        <v>552</v>
+        <v>5456</v>
       </c>
       <c r="S19" s="2">
-        <v>24283.1</v>
+        <v>41571.199999999997</v>
       </c>
       <c r="T19" s="2">
-        <v>992.7</v>
+        <v>2116</v>
       </c>
       <c r="U19" s="2">
-        <v>-258</v>
+        <v>704</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1246,152 +1288,42 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C20" s="2">
-        <v>81.863</v>
+        <v>82.691999999999993</v>
       </c>
       <c r="D20" s="2">
-        <v>29</v>
+        <v>30.728999999999999</v>
       </c>
       <c r="E20" s="2">
-        <v>929</v>
+        <v>643</v>
       </c>
       <c r="F20" s="2">
-        <v>42361</v>
-      </c>
-      <c r="G20" s="2"/>
+        <v>49270</v>
+      </c>
       <c r="H20" s="2">
         <v>8508</v>
       </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2">
-        <v>26447.994999999999</v>
-      </c>
-      <c r="M20" s="2"/>
       <c r="N20" s="2">
-        <v>3334</v>
+        <v>3373</v>
       </c>
       <c r="O20" s="2">
-        <v>3321.5</v>
-      </c>
-      <c r="P20" s="2">
-        <v>150.80000000000001</v>
+        <v>5465.4</v>
       </c>
       <c r="Q20" s="2">
-        <v>532.51300000000003</v>
+        <v>592.06500000000005</v>
       </c>
       <c r="R20" s="2">
-        <v>5456</v>
+        <v>7363</v>
       </c>
       <c r="S20" s="2">
-        <v>41571.199999999997</v>
+        <v>49034.2</v>
       </c>
       <c r="T20" s="2">
-        <v>2116</v>
+        <v>3455.4180000000001</v>
       </c>
       <c r="U20" s="2">
-        <v>704</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C21" s="2">
-        <v>80.203999999999994</v>
-      </c>
-      <c r="D21" s="2">
-        <v>18.2</v>
-      </c>
-      <c r="E21" s="2">
-        <v>212</v>
-      </c>
-      <c r="F21" s="2">
-        <v>48384</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2">
-        <v>5843</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2">
-        <v>7713.7349999999997</v>
-      </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2">
-        <v>2489</v>
-      </c>
-      <c r="O21" s="2">
-        <v>2937.3</v>
-      </c>
-      <c r="P21" s="2">
-        <v>3009</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>188.37</v>
-      </c>
-      <c r="R21" s="2">
-        <v>970</v>
-      </c>
-      <c r="S21" s="2">
-        <v>27967.1</v>
-      </c>
-      <c r="T21" s="2">
-        <v>631.20000000000005</v>
-      </c>
-      <c r="U21" s="2">
-        <v>-366</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="2">
-        <v>2023</v>
-      </c>
-      <c r="C22" s="2">
-        <v>82.691999999999993</v>
-      </c>
-      <c r="D22" s="2">
-        <v>30.728999999999999</v>
-      </c>
-      <c r="E22" s="2">
-        <v>643</v>
-      </c>
-      <c r="F22" s="2">
-        <v>49270</v>
-      </c>
-      <c r="H22" s="2">
-        <v>8508</v>
-      </c>
-      <c r="N22" s="2">
-        <v>3373</v>
-      </c>
-      <c r="O22" s="2">
-        <v>5465.4</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>592.06500000000005</v>
-      </c>
-      <c r="R22" s="2">
-        <v>7363</v>
-      </c>
-      <c r="S22" s="2">
-        <v>49034.2</v>
-      </c>
-      <c r="T22" s="2">
-        <v>3455.4180000000001</v>
-      </c>
-      <c r="U22" s="2">
         <v>4899</v>
       </c>
     </row>
@@ -1400,45 +1332,191 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C23" s="2">
+        <v>76.783000000000001</v>
+      </c>
+      <c r="D23" s="2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E23" s="2">
+        <v>894</v>
+      </c>
+      <c r="F23" s="2">
+        <v>37974</v>
+      </c>
+      <c r="N23" s="2">
+        <v>2586</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1326.7</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1094.7</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>74.545000000000002</v>
+      </c>
+      <c r="R23" s="2">
+        <v>416</v>
+      </c>
+      <c r="S23" s="2">
+        <v>17282</v>
+      </c>
+      <c r="T23" s="2">
+        <v>1027.8</v>
+      </c>
+      <c r="U23" s="2">
+        <v>-1278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C24" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D24" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E24" s="2">
+        <v>262</v>
+      </c>
+      <c r="F24" s="2">
+        <v>42904</v>
+      </c>
+      <c r="L24">
+        <v>10326.647999999999</v>
+      </c>
+      <c r="N24" s="2">
+        <v>2565</v>
+      </c>
+      <c r="O24" s="2">
+        <v>1318.4</v>
+      </c>
+      <c r="P24" s="2">
+        <v>4092.5</v>
+      </c>
+      <c r="Q24" s="2">
+        <v>101.312</v>
+      </c>
+      <c r="R24" s="2">
+        <v>552</v>
+      </c>
+      <c r="S24" s="2">
+        <v>24283.1</v>
+      </c>
+      <c r="T24" s="2">
+        <v>992.7</v>
+      </c>
+      <c r="U24" s="2">
+        <v>-258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C25" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D25" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E25" s="2">
+        <v>212</v>
+      </c>
+      <c r="F25" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2">
+        <v>5843</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2">
+        <v>7713.7349999999997</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O25" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P25" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q25" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R25" s="2">
+        <v>970</v>
+      </c>
+      <c r="S25" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T25" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U25" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="2">
         <v>2023</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C26" s="2">
         <v>80.296000000000006</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D26" s="2">
         <v>19.093</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E26" s="2">
         <v>96</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F26" s="2">
         <v>56182</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H26" s="2">
         <v>5703</v>
       </c>
-      <c r="N23" s="2">
+      <c r="N26" s="2">
         <v>2396</v>
       </c>
-      <c r="O23" s="2">
+      <c r="O26" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P26" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q23" s="2">
+      <c r="Q26" s="2">
         <v>114.619</v>
       </c>
-      <c r="R23" s="2">
+      <c r="R26" s="2">
         <v>646</v>
       </c>
-      <c r="S23" s="2">
+      <c r="S26" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T26" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U23" s="2">
+      <c r="U26" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Anapa, GL, Gelen. 2019 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -441,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U26"/>
+  <dimension ref="A1:U27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -921,6 +921,9 @@
       <c r="T10" s="2">
         <v>22.9</v>
       </c>
+      <c r="U10" s="2">
+        <v>1872</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
@@ -932,17 +935,38 @@
       <c r="C11" s="2">
         <v>38.972000000000001</v>
       </c>
+      <c r="D11" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="E11" s="2">
+        <v>267</v>
+      </c>
       <c r="F11" s="2">
         <v>34491</v>
       </c>
+      <c r="N11" s="2">
+        <v>942</v>
+      </c>
       <c r="O11" s="2">
         <v>2533.6999999999998</v>
       </c>
+      <c r="P11" s="2">
+        <v>94.8</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>73.932000000000002</v>
+      </c>
+      <c r="R11" s="2">
+        <v>1157</v>
+      </c>
       <c r="S11" s="2">
         <v>46733.5</v>
       </c>
       <c r="T11" s="2">
         <v>22.4</v>
+      </c>
+      <c r="U11" s="2">
+        <v>1717</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -1137,48 +1161,53 @@
         <v>1165</v>
       </c>
     </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2018</v>
+      </c>
+    </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C17" s="2">
-        <v>88.879000000000005</v>
+        <v>2019</v>
       </c>
       <c r="D17" s="2">
-        <v>26.6</v>
+        <v>26</v>
       </c>
       <c r="E17" s="2">
-        <v>5378</v>
+        <v>743</v>
       </c>
       <c r="F17" s="2">
-        <v>34049</v>
+        <v>33185</v>
       </c>
       <c r="N17" s="2">
-        <v>3562</v>
+        <v>3822</v>
       </c>
       <c r="O17" s="2">
-        <v>1845</v>
+        <v>1871.8</v>
       </c>
       <c r="P17" s="2">
-        <v>637.29999999999995</v>
+        <v>3351.1</v>
       </c>
       <c r="Q17" s="2">
-        <v>526.50900000000001</v>
+        <v>484.16899999999998</v>
       </c>
       <c r="R17" s="2">
-        <v>9241</v>
+        <v>9054</v>
       </c>
       <c r="S17" s="2">
-        <v>26593</v>
+        <v>23432.799999999999</v>
       </c>
       <c r="T17" s="2">
-        <v>753.2</v>
+        <v>749.8</v>
       </c>
       <c r="U17" s="2">
-        <v>7130</v>
+        <v>10533</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1186,46 +1215,43 @@
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C18" s="2">
-        <v>81.863</v>
+        <v>88.879000000000005</v>
       </c>
       <c r="D18" s="2">
-        <v>28.3</v>
+        <v>26.6</v>
       </c>
       <c r="E18" s="2">
-        <v>1017</v>
+        <v>5378</v>
       </c>
       <c r="F18" s="2">
-        <v>38808</v>
-      </c>
-      <c r="L18">
-        <v>15703.486000000001</v>
+        <v>34049</v>
       </c>
       <c r="N18" s="2">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="O18" s="2">
-        <v>2466.6999999999998</v>
+        <v>1845</v>
       </c>
       <c r="P18" s="2">
-        <v>289.2</v>
+        <v>637.29999999999995</v>
       </c>
       <c r="Q18" s="2">
-        <v>523.16399999999999</v>
+        <v>526.50900000000001</v>
       </c>
       <c r="R18" s="2">
-        <v>8415</v>
+        <v>9241</v>
       </c>
       <c r="S18" s="2">
-        <v>36829.599999999999</v>
+        <v>26593</v>
       </c>
       <c r="T18" s="2">
-        <v>1014.6</v>
+        <v>753.2</v>
       </c>
       <c r="U18" s="2">
-        <v>1556</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1233,54 +1259,46 @@
         <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C19" s="2">
         <v>81.863</v>
       </c>
       <c r="D19" s="2">
-        <v>29</v>
+        <v>28.3</v>
       </c>
       <c r="E19" s="2">
-        <v>929</v>
+        <v>1017</v>
       </c>
       <c r="F19" s="2">
-        <v>42361</v>
-      </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2">
-        <v>8508</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2">
-        <v>26447.994999999999</v>
-      </c>
-      <c r="M19" s="2"/>
+        <v>38808</v>
+      </c>
+      <c r="L19">
+        <v>15703.486000000001</v>
+      </c>
       <c r="N19" s="2">
-        <v>3334</v>
+        <v>3561</v>
       </c>
       <c r="O19" s="2">
-        <v>3321.5</v>
+        <v>2466.6999999999998</v>
       </c>
       <c r="P19" s="2">
-        <v>150.80000000000001</v>
+        <v>289.2</v>
       </c>
       <c r="Q19" s="2">
-        <v>532.51300000000003</v>
+        <v>523.16399999999999</v>
       </c>
       <c r="R19" s="2">
-        <v>5456</v>
+        <v>8415</v>
       </c>
       <c r="S19" s="2">
-        <v>41571.199999999997</v>
+        <v>36829.599999999999</v>
       </c>
       <c r="T19" s="2">
-        <v>2116</v>
+        <v>1014.6</v>
       </c>
       <c r="U19" s="2">
-        <v>704</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1288,43 +1306,106 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C20" s="2">
-        <v>82.691999999999993</v>
+        <v>81.863</v>
       </c>
       <c r="D20" s="2">
-        <v>30.728999999999999</v>
+        <v>29</v>
       </c>
       <c r="E20" s="2">
-        <v>643</v>
+        <v>929</v>
       </c>
       <c r="F20" s="2">
-        <v>49270</v>
-      </c>
+        <v>42361</v>
+      </c>
+      <c r="G20" s="2"/>
       <c r="H20" s="2">
         <v>8508</v>
       </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2">
+        <v>26447.994999999999</v>
+      </c>
+      <c r="M20" s="2"/>
       <c r="N20" s="2">
+        <v>3334</v>
+      </c>
+      <c r="O20" s="2">
+        <v>3321.5</v>
+      </c>
+      <c r="P20" s="2">
+        <v>150.80000000000001</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>532.51300000000003</v>
+      </c>
+      <c r="R20" s="2">
+        <v>5456</v>
+      </c>
+      <c r="S20" s="2">
+        <v>41571.199999999997</v>
+      </c>
+      <c r="T20" s="2">
+        <v>2116</v>
+      </c>
+      <c r="U20" s="2">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C21" s="2">
+        <v>82.691999999999993</v>
+      </c>
+      <c r="D21" s="2">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="E21" s="2">
+        <v>643</v>
+      </c>
+      <c r="F21" s="2">
+        <v>49270</v>
+      </c>
+      <c r="H21" s="2">
+        <v>8508</v>
+      </c>
+      <c r="N21" s="2">
         <v>3373</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O21" s="2">
         <v>5465.4</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q21" s="2">
         <v>592.06500000000005</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R21" s="2">
         <v>7363</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S21" s="2">
         <v>49034.2</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T21" s="2">
         <v>3455.4180000000001</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U21" s="2">
         <v>4899</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2018</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -1332,43 +1413,40 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C23" s="2">
-        <v>76.783000000000001</v>
+        <v>2019</v>
       </c>
       <c r="D23" s="2">
-        <v>17.600000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="E23" s="2">
-        <v>894</v>
+        <v>266</v>
       </c>
       <c r="F23" s="2">
-        <v>37974</v>
+        <v>36573</v>
       </c>
       <c r="N23" s="2">
-        <v>2586</v>
+        <v>2717</v>
       </c>
       <c r="O23" s="2">
-        <v>1326.7</v>
+        <v>2218.6999999999998</v>
       </c>
       <c r="P23" s="2">
-        <v>1094.7</v>
+        <v>200.3</v>
       </c>
       <c r="Q23" s="2">
-        <v>74.545000000000002</v>
+        <v>85.382999999999996</v>
       </c>
       <c r="R23" s="2">
-        <v>416</v>
+        <v>915</v>
       </c>
       <c r="S23" s="2">
-        <v>17282</v>
+        <v>14798.4</v>
       </c>
       <c r="T23" s="2">
-        <v>1027.8</v>
+        <v>878.2</v>
       </c>
       <c r="U23" s="2">
-        <v>-1278</v>
+        <v>-553</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -1376,46 +1454,43 @@
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C24" s="2">
-        <v>80.203999999999994</v>
+        <v>76.783000000000001</v>
       </c>
       <c r="D24" s="2">
-        <v>18.600000000000001</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E24" s="2">
-        <v>262</v>
+        <v>894</v>
       </c>
       <c r="F24" s="2">
-        <v>42904</v>
-      </c>
-      <c r="L24">
-        <v>10326.647999999999</v>
+        <v>37974</v>
       </c>
       <c r="N24" s="2">
-        <v>2565</v>
+        <v>2586</v>
       </c>
       <c r="O24" s="2">
-        <v>1318.4</v>
+        <v>1326.7</v>
       </c>
       <c r="P24" s="2">
-        <v>4092.5</v>
+        <v>1094.7</v>
       </c>
       <c r="Q24" s="2">
-        <v>101.312</v>
+        <v>74.545000000000002</v>
       </c>
       <c r="R24" s="2">
-        <v>552</v>
+        <v>416</v>
       </c>
       <c r="S24" s="2">
-        <v>24283.1</v>
+        <v>17282</v>
       </c>
       <c r="T24" s="2">
-        <v>992.7</v>
+        <v>1027.8</v>
       </c>
       <c r="U24" s="2">
-        <v>-258</v>
+        <v>-1278</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -1423,54 +1498,46 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C25" s="2">
         <v>80.203999999999994</v>
       </c>
       <c r="D25" s="2">
-        <v>18.2</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="E25" s="2">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="F25" s="2">
-        <v>48384</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2">
-        <v>5843</v>
-      </c>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2">
-        <v>7713.7349999999997</v>
-      </c>
-      <c r="M25" s="2"/>
+        <v>42904</v>
+      </c>
+      <c r="L25">
+        <v>10326.647999999999</v>
+      </c>
       <c r="N25" s="2">
-        <v>2489</v>
+        <v>2565</v>
       </c>
       <c r="O25" s="2">
-        <v>2937.3</v>
+        <v>1318.4</v>
       </c>
       <c r="P25" s="2">
-        <v>3009</v>
+        <v>4092.5</v>
       </c>
       <c r="Q25" s="2">
-        <v>188.37</v>
+        <v>101.312</v>
       </c>
       <c r="R25" s="2">
-        <v>970</v>
+        <v>552</v>
       </c>
       <c r="S25" s="2">
-        <v>27967.1</v>
+        <v>24283.1</v>
       </c>
       <c r="T25" s="2">
-        <v>631.20000000000005</v>
+        <v>992.7</v>
       </c>
       <c r="U25" s="2">
-        <v>-366</v>
+        <v>-258</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -1478,45 +1545,100 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C26" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D26" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E26" s="2">
+        <v>212</v>
+      </c>
+      <c r="F26" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <v>5843</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2">
+        <v>7713.7349999999997</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O26" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P26" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R26" s="2">
+        <v>970</v>
+      </c>
+      <c r="S26" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T26" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U26" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="2">
         <v>2023</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C27" s="2">
         <v>80.296000000000006</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D27" s="2">
         <v>19.093</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E27" s="2">
         <v>96</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F27" s="2">
         <v>56182</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H27" s="2">
         <v>5703</v>
       </c>
-      <c r="N26" s="2">
+      <c r="N27" s="2">
         <v>2396</v>
       </c>
-      <c r="O26" s="2">
+      <c r="O27" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P26" s="2">
+      <c r="P27" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q26" s="2">
+      <c r="Q27" s="2">
         <v>114.619</v>
       </c>
-      <c r="R26" s="2">
+      <c r="R27" s="2">
         <v>646</v>
       </c>
-      <c r="S26" s="2">
+      <c r="S27" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T26" s="2">
+      <c r="T27" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U26" s="2">
+      <c r="U27" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Anapa, GK, Gelen. 2018 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -118,18 +118,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,10 +149,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -441,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U27"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,14 +900,29 @@
       <c r="C10" s="2">
         <v>37.475000000000001</v>
       </c>
+      <c r="D10" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E10" s="2">
+        <v>216</v>
+      </c>
       <c r="F10" s="2">
         <v>31404</v>
       </c>
+      <c r="N10" s="2">
+        <v>996</v>
+      </c>
       <c r="O10" s="2">
         <v>3495.3</v>
       </c>
       <c r="P10" s="2">
         <v>94.3</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>72.433000000000007</v>
+      </c>
+      <c r="R10" s="2">
+        <v>982</v>
       </c>
       <c r="S10" s="2">
         <v>46980</v>
@@ -1166,7 +1175,10 @@
         <v>23</v>
       </c>
       <c r="B16" s="2">
-        <v>2018</v>
+        <v>2017</v>
+      </c>
+      <c r="U16" s="2">
+        <v>-677</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
@@ -1174,40 +1186,40 @@
         <v>23</v>
       </c>
       <c r="B17" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="D17" s="2">
-        <v>26</v>
+        <v>24.9</v>
       </c>
       <c r="E17" s="2">
-        <v>743</v>
+        <v>507</v>
       </c>
       <c r="F17" s="2">
-        <v>33185</v>
+        <v>31629</v>
       </c>
       <c r="N17" s="2">
-        <v>3822</v>
+        <v>4471</v>
       </c>
       <c r="O17" s="2">
-        <v>1871.8</v>
+        <v>1435.5</v>
       </c>
       <c r="P17" s="2">
-        <v>3351.1</v>
+        <v>4022.4</v>
       </c>
       <c r="Q17" s="2">
-        <v>484.16899999999998</v>
+        <v>422.51900000000001</v>
       </c>
       <c r="R17" s="2">
-        <v>9054</v>
+        <v>7064</v>
       </c>
       <c r="S17" s="2">
-        <v>23432.799999999999</v>
+        <v>20304.5</v>
       </c>
       <c r="T17" s="2">
-        <v>749.8</v>
+        <v>389.4</v>
       </c>
       <c r="U17" s="2">
-        <v>10533</v>
+        <v>7470</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
@@ -1215,43 +1227,40 @@
         <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C18" s="2">
-        <v>88.879000000000005</v>
+        <v>2019</v>
       </c>
       <c r="D18" s="2">
-        <v>26.6</v>
+        <v>26</v>
       </c>
       <c r="E18" s="2">
-        <v>5378</v>
+        <v>743</v>
       </c>
       <c r="F18" s="2">
-        <v>34049</v>
+        <v>33185</v>
       </c>
       <c r="N18" s="2">
-        <v>3562</v>
+        <v>3822</v>
       </c>
       <c r="O18" s="2">
-        <v>1845</v>
+        <v>1871.8</v>
       </c>
       <c r="P18" s="2">
-        <v>637.29999999999995</v>
+        <v>3351.1</v>
       </c>
       <c r="Q18" s="2">
-        <v>526.50900000000001</v>
+        <v>484.16899999999998</v>
       </c>
       <c r="R18" s="2">
-        <v>9241</v>
+        <v>9054</v>
       </c>
       <c r="S18" s="2">
-        <v>26593</v>
+        <v>23432.799999999999</v>
       </c>
       <c r="T18" s="2">
-        <v>753.2</v>
+        <v>749.8</v>
       </c>
       <c r="U18" s="2">
-        <v>7130</v>
+        <v>10533</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
@@ -1259,46 +1268,43 @@
         <v>23</v>
       </c>
       <c r="B19" s="2">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="C19" s="2">
-        <v>81.863</v>
+        <v>88.879000000000005</v>
       </c>
       <c r="D19" s="2">
-        <v>28.3</v>
+        <v>26.6</v>
       </c>
       <c r="E19" s="2">
-        <v>1017</v>
+        <v>5378</v>
       </c>
       <c r="F19" s="2">
-        <v>38808</v>
-      </c>
-      <c r="L19">
-        <v>15703.486000000001</v>
+        <v>34049</v>
       </c>
       <c r="N19" s="2">
-        <v>3561</v>
+        <v>3562</v>
       </c>
       <c r="O19" s="2">
-        <v>2466.6999999999998</v>
+        <v>1845</v>
       </c>
       <c r="P19" s="2">
-        <v>289.2</v>
+        <v>637.29999999999995</v>
       </c>
       <c r="Q19" s="2">
-        <v>523.16399999999999</v>
+        <v>526.50900000000001</v>
       </c>
       <c r="R19" s="2">
-        <v>8415</v>
+        <v>9241</v>
       </c>
       <c r="S19" s="2">
-        <v>36829.599999999999</v>
+        <v>26593</v>
       </c>
       <c r="T19" s="2">
-        <v>1014.6</v>
+        <v>753.2</v>
       </c>
       <c r="U19" s="2">
-        <v>1556</v>
+        <v>7130</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
@@ -1306,54 +1312,46 @@
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="C20" s="2">
         <v>81.863</v>
       </c>
       <c r="D20" s="2">
-        <v>29</v>
+        <v>28.3</v>
       </c>
       <c r="E20" s="2">
-        <v>929</v>
+        <v>1017</v>
       </c>
       <c r="F20" s="2">
-        <v>42361</v>
-      </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2">
-        <v>8508</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2">
-        <v>26447.994999999999</v>
-      </c>
-      <c r="M20" s="2"/>
+        <v>38808</v>
+      </c>
+      <c r="L20">
+        <v>15703.486000000001</v>
+      </c>
       <c r="N20" s="2">
-        <v>3334</v>
+        <v>3561</v>
       </c>
       <c r="O20" s="2">
-        <v>3321.5</v>
+        <v>2466.6999999999998</v>
       </c>
       <c r="P20" s="2">
-        <v>150.80000000000001</v>
+        <v>289.2</v>
       </c>
       <c r="Q20" s="2">
-        <v>532.51300000000003</v>
+        <v>523.16399999999999</v>
       </c>
       <c r="R20" s="2">
-        <v>5456</v>
+        <v>8415</v>
       </c>
       <c r="S20" s="2">
-        <v>41571.199999999997</v>
+        <v>36829.599999999999</v>
       </c>
       <c r="T20" s="2">
-        <v>2116</v>
+        <v>1014.6</v>
       </c>
       <c r="U20" s="2">
-        <v>704</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
@@ -1361,51 +1359,98 @@
         <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="C21" s="2">
-        <v>82.691999999999993</v>
+        <v>81.863</v>
       </c>
       <c r="D21" s="2">
-        <v>30.728999999999999</v>
+        <v>29</v>
       </c>
       <c r="E21" s="2">
-        <v>643</v>
+        <v>929</v>
       </c>
       <c r="F21" s="2">
-        <v>49270</v>
-      </c>
+        <v>42361</v>
+      </c>
+      <c r="G21" s="2"/>
       <c r="H21" s="2">
         <v>8508</v>
       </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2">
+        <v>26447.994999999999</v>
+      </c>
+      <c r="M21" s="2"/>
       <c r="N21" s="2">
-        <v>3373</v>
+        <v>3334</v>
       </c>
       <c r="O21" s="2">
-        <v>5465.4</v>
+        <v>3321.5</v>
+      </c>
+      <c r="P21" s="2">
+        <v>150.80000000000001</v>
       </c>
       <c r="Q21" s="2">
-        <v>592.06500000000005</v>
+        <v>532.51300000000003</v>
       </c>
       <c r="R21" s="2">
-        <v>7363</v>
+        <v>5456</v>
       </c>
       <c r="S21" s="2">
-        <v>49034.2</v>
+        <v>41571.199999999997</v>
       </c>
       <c r="T21" s="2">
-        <v>3455.4180000000001</v>
+        <v>2116</v>
       </c>
       <c r="U21" s="2">
-        <v>4899</v>
+        <v>704</v>
       </c>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" s="2">
-        <v>2018</v>
+        <v>2023</v>
+      </c>
+      <c r="C22" s="2">
+        <v>82.691999999999993</v>
+      </c>
+      <c r="D22" s="2">
+        <v>30.728999999999999</v>
+      </c>
+      <c r="E22" s="2">
+        <v>643</v>
+      </c>
+      <c r="F22" s="2">
+        <v>49270</v>
+      </c>
+      <c r="H22" s="2">
+        <v>8508</v>
+      </c>
+      <c r="N22" s="2">
+        <v>3373</v>
+      </c>
+      <c r="O22" s="2">
+        <v>5465.4</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>592.06500000000005</v>
+      </c>
+      <c r="R22" s="2">
+        <v>7363</v>
+      </c>
+      <c r="S22" s="2">
+        <v>49034.2</v>
+      </c>
+      <c r="T22" s="2">
+        <v>3455.4180000000001</v>
+      </c>
+      <c r="U22" s="2">
+        <v>4899</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
@@ -1413,40 +1458,10 @@
         <v>24</v>
       </c>
       <c r="B23" s="2">
-        <v>2019</v>
-      </c>
-      <c r="D23" s="2">
-        <v>17.2</v>
-      </c>
-      <c r="E23" s="2">
-        <v>266</v>
-      </c>
-      <c r="F23" s="2">
-        <v>36573</v>
-      </c>
-      <c r="N23" s="2">
-        <v>2717</v>
-      </c>
-      <c r="O23" s="2">
-        <v>2218.6999999999998</v>
-      </c>
-      <c r="P23" s="2">
-        <v>200.3</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>85.382999999999996</v>
-      </c>
-      <c r="R23" s="2">
-        <v>915</v>
-      </c>
-      <c r="S23" s="2">
-        <v>14798.4</v>
-      </c>
-      <c r="T23" s="2">
-        <v>878.2</v>
+        <v>2017</v>
       </c>
       <c r="U23" s="2">
-        <v>-553</v>
+        <v>2138</v>
       </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
@@ -1454,43 +1469,40 @@
         <v>24</v>
       </c>
       <c r="B24" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C24" s="2">
-        <v>76.783000000000001</v>
+        <v>2018</v>
       </c>
       <c r="D24" s="2">
-        <v>17.600000000000001</v>
+        <v>17</v>
       </c>
       <c r="E24" s="2">
-        <v>894</v>
+        <v>196</v>
       </c>
       <c r="F24" s="2">
-        <v>37974</v>
+        <v>33853</v>
       </c>
       <c r="N24" s="2">
-        <v>2586</v>
+        <v>3047</v>
       </c>
       <c r="O24" s="2">
-        <v>1326.7</v>
+        <v>1997.1</v>
       </c>
       <c r="P24" s="2">
-        <v>1094.7</v>
+        <v>174.9</v>
       </c>
       <c r="Q24" s="2">
-        <v>74.545000000000002</v>
+        <v>111.617</v>
       </c>
       <c r="R24" s="2">
-        <v>416</v>
+        <v>1622</v>
       </c>
       <c r="S24" s="2">
-        <v>17282</v>
+        <v>13072.3</v>
       </c>
       <c r="T24" s="2">
-        <v>1027.8</v>
+        <v>753.8</v>
       </c>
       <c r="U24" s="2">
-        <v>-1278</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
@@ -1498,46 +1510,40 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C25" s="2">
-        <v>80.203999999999994</v>
+        <v>2019</v>
       </c>
       <c r="D25" s="2">
-        <v>18.600000000000001</v>
+        <v>17.2</v>
       </c>
       <c r="E25" s="2">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="F25" s="2">
-        <v>42904</v>
-      </c>
-      <c r="L25">
-        <v>10326.647999999999</v>
+        <v>36573</v>
       </c>
       <c r="N25" s="2">
-        <v>2565</v>
+        <v>2717</v>
       </c>
       <c r="O25" s="2">
-        <v>1318.4</v>
+        <v>2218.6999999999998</v>
       </c>
       <c r="P25" s="2">
-        <v>4092.5</v>
+        <v>200.3</v>
       </c>
       <c r="Q25" s="2">
-        <v>101.312</v>
+        <v>85.382999999999996</v>
       </c>
       <c r="R25" s="2">
-        <v>552</v>
+        <v>915</v>
       </c>
       <c r="S25" s="2">
-        <v>24283.1</v>
+        <v>14798.4</v>
       </c>
       <c r="T25" s="2">
-        <v>992.7</v>
+        <v>878.2</v>
       </c>
       <c r="U25" s="2">
-        <v>-258</v>
+        <v>-553</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
@@ -1545,54 +1551,43 @@
         <v>24</v>
       </c>
       <c r="B26" s="2">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C26" s="2">
-        <v>80.203999999999994</v>
+        <v>76.783000000000001</v>
       </c>
       <c r="D26" s="2">
-        <v>18.2</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E26" s="2">
-        <v>212</v>
+        <v>894</v>
       </c>
       <c r="F26" s="2">
-        <v>48384</v>
-      </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2">
-        <v>5843</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2">
-        <v>7713.7349999999997</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>37974</v>
+      </c>
       <c r="N26" s="2">
-        <v>2489</v>
+        <v>2586</v>
       </c>
       <c r="O26" s="2">
-        <v>2937.3</v>
+        <v>1326.7</v>
       </c>
       <c r="P26" s="2">
-        <v>3009</v>
+        <v>1094.7</v>
       </c>
       <c r="Q26" s="2">
-        <v>188.37</v>
+        <v>74.545000000000002</v>
       </c>
       <c r="R26" s="2">
-        <v>970</v>
+        <v>416</v>
       </c>
       <c r="S26" s="2">
-        <v>27967.1</v>
+        <v>17282</v>
       </c>
       <c r="T26" s="2">
-        <v>631.20000000000005</v>
+        <v>1027.8</v>
       </c>
       <c r="U26" s="2">
-        <v>-366</v>
+        <v>-1278</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
@@ -1600,45 +1595,147 @@
         <v>24</v>
       </c>
       <c r="B27" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C27" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D27" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E27" s="2">
+        <v>262</v>
+      </c>
+      <c r="F27" s="2">
+        <v>42904</v>
+      </c>
+      <c r="L27">
+        <v>10326.647999999999</v>
+      </c>
+      <c r="N27" s="2">
+        <v>2565</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1318.4</v>
+      </c>
+      <c r="P27" s="2">
+        <v>4092.5</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>101.312</v>
+      </c>
+      <c r="R27" s="2">
+        <v>552</v>
+      </c>
+      <c r="S27" s="2">
+        <v>24283.1</v>
+      </c>
+      <c r="T27" s="2">
+        <v>992.7</v>
+      </c>
+      <c r="U27" s="2">
+        <v>-258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C28" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D28" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>212</v>
+      </c>
+      <c r="F28" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2">
+        <v>5843</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2">
+        <v>7713.7349999999997</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O28" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P28" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R28" s="2">
+        <v>970</v>
+      </c>
+      <c r="S28" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T28" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U28" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" s="2">
         <v>2023</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C29" s="2">
         <v>80.296000000000006</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D29" s="2">
         <v>19.093</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E29" s="2">
         <v>96</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F29" s="2">
         <v>56182</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H29" s="2">
         <v>5703</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N29" s="2">
         <v>2396</v>
       </c>
-      <c r="O27" s="2">
+      <c r="O29" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P27" s="2">
+      <c r="P29" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q27" s="2">
+      <c r="Q29" s="2">
         <v>114.619</v>
       </c>
-      <c r="R27" s="2">
+      <c r="R29" s="2">
         <v>646</v>
       </c>
-      <c r="S27" s="2">
+      <c r="S29" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T27" s="2">
+      <c r="T29" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U27" s="2">
+      <c r="U29" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Anapa, GK, Gelen. 2017 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/less100/kraskray.xlsx
+++ b/migforecasting/less100/kraskray.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -118,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -138,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -155,6 +161,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -435,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -891,91 +901,81 @@
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="2">
-        <v>2018</v>
-      </c>
-      <c r="C10" s="2">
-        <v>37.475000000000001</v>
-      </c>
-      <c r="D10" s="2">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="E10" s="2">
-        <v>216</v>
-      </c>
-      <c r="F10" s="2">
-        <v>31404</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="B10" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="4">
+        <v>2017</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E11" s="4">
+        <v>241</v>
+      </c>
+      <c r="F11" s="4">
+        <v>30134</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4">
         <v>996</v>
       </c>
-      <c r="O10" s="2">
-        <v>3495.3</v>
-      </c>
-      <c r="P10" s="2">
-        <v>94.3</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>72.433000000000007</v>
-      </c>
-      <c r="R10" s="2">
-        <v>982</v>
-      </c>
-      <c r="S10" s="2">
-        <v>46980</v>
-      </c>
-      <c r="T10" s="2">
-        <v>22.9</v>
-      </c>
-      <c r="U10" s="2">
-        <v>1872</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="2">
-        <v>2019</v>
-      </c>
-      <c r="C11" s="2">
-        <v>38.972000000000001</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8.4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>267</v>
-      </c>
-      <c r="F11" s="2">
-        <v>34491</v>
-      </c>
-      <c r="N11" s="2">
-        <v>942</v>
-      </c>
-      <c r="O11" s="2">
-        <v>2533.6999999999998</v>
-      </c>
-      <c r="P11" s="2">
-        <v>94.8</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>73.932000000000002</v>
-      </c>
-      <c r="R11" s="2">
-        <v>1157</v>
-      </c>
-      <c r="S11" s="2">
-        <v>46733.5</v>
-      </c>
-      <c r="T11" s="2">
-        <v>22.4</v>
-      </c>
-      <c r="U11" s="2">
-        <v>1717</v>
+      <c r="O11" s="4">
+        <v>3388.6</v>
+      </c>
+      <c r="P11" s="4">
+        <v>129.9</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>58.734000000000002</v>
+      </c>
+      <c r="R11" s="4">
+        <v>766</v>
+      </c>
+      <c r="S11" s="4">
+        <v>30213.200000000001</v>
+      </c>
+      <c r="T11" s="4">
+        <v>10.6</v>
+      </c>
+      <c r="U11" s="4">
+        <v>955</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -983,43 +983,43 @@
         <v>22</v>
       </c>
       <c r="B12" s="2">
-        <v>2020</v>
+        <v>2018</v>
       </c>
       <c r="C12" s="2">
-        <v>40.298999999999999</v>
+        <v>37.475000000000001</v>
       </c>
       <c r="D12" s="2">
-        <v>8.9</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="E12" s="2">
-        <v>799</v>
+        <v>216</v>
       </c>
       <c r="F12" s="2">
-        <v>38996</v>
+        <v>31404</v>
       </c>
       <c r="N12" s="2">
-        <v>880</v>
+        <v>996</v>
       </c>
       <c r="O12" s="2">
-        <v>2392.9</v>
+        <v>3495.3</v>
       </c>
       <c r="P12" s="2">
-        <v>117.2</v>
+        <v>94.3</v>
       </c>
       <c r="Q12" s="2">
-        <v>66.64</v>
+        <v>72.433000000000007</v>
       </c>
       <c r="R12" s="2">
-        <v>990</v>
+        <v>982</v>
       </c>
       <c r="S12" s="2">
-        <v>50203.3</v>
+        <v>46980</v>
       </c>
       <c r="T12" s="2">
-        <v>61.8</v>
+        <v>22.9</v>
       </c>
       <c r="U12" s="2">
-        <v>2003</v>
+        <v>1872</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -1027,46 +1027,43 @@
         <v>22</v>
       </c>
       <c r="B13" s="2">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="C13" s="2">
-        <v>40.902999999999999</v>
+        <v>38.972000000000001</v>
       </c>
       <c r="D13" s="2">
-        <v>8.1999999999999993</v>
+        <v>8.4</v>
       </c>
       <c r="E13" s="2">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="F13" s="2">
-        <v>35126.300000000003</v>
-      </c>
-      <c r="L13">
-        <v>1384.127</v>
+        <v>34491</v>
       </c>
       <c r="N13" s="2">
-        <v>850</v>
+        <v>942</v>
       </c>
       <c r="O13" s="2">
-        <v>2665.5</v>
+        <v>2533.6999999999998</v>
       </c>
       <c r="P13" s="2">
-        <v>151.80000000000001</v>
+        <v>94.8</v>
       </c>
       <c r="Q13" s="2">
-        <v>76.257999999999996</v>
+        <v>73.932000000000002</v>
       </c>
       <c r="R13" s="2">
-        <v>1089</v>
+        <v>1157</v>
       </c>
       <c r="S13" s="2">
-        <v>26942.7</v>
+        <v>46733.5</v>
       </c>
       <c r="T13" s="2">
-        <v>91.8</v>
+        <v>22.4</v>
       </c>
       <c r="U13" s="2">
-        <v>1529</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -1074,49 +1071,43 @@
         <v>22</v>
       </c>
       <c r="B14" s="2">
-        <v>2022</v>
+        <v>2020</v>
       </c>
       <c r="C14" s="2">
-        <v>41</v>
+        <v>40.298999999999999</v>
       </c>
       <c r="D14" s="2">
-        <v>8.5</v>
+        <v>8.9</v>
       </c>
       <c r="E14" s="2">
-        <v>225</v>
+        <v>799</v>
       </c>
       <c r="F14" s="2">
-        <v>38166</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2544</v>
-      </c>
-      <c r="L14">
-        <v>863.57799999999997</v>
+        <v>38996</v>
       </c>
       <c r="N14" s="2">
-        <v>873</v>
+        <v>880</v>
       </c>
       <c r="O14" s="2">
-        <v>3265.1</v>
+        <v>2392.9</v>
       </c>
       <c r="P14" s="2">
-        <v>213.9</v>
+        <v>117.2</v>
       </c>
       <c r="Q14" s="2">
-        <v>85.277000000000001</v>
+        <v>66.64</v>
       </c>
       <c r="R14" s="2">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="S14" s="2">
-        <v>15205.4</v>
+        <v>50203.3</v>
       </c>
       <c r="T14" s="2">
-        <v>466.7</v>
+        <v>61.8</v>
       </c>
       <c r="U14" s="2">
-        <v>1148</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1124,618 +1115,921 @@
         <v>22</v>
       </c>
       <c r="B15" s="2">
-        <v>2023</v>
+        <v>2021</v>
       </c>
       <c r="C15" s="2">
-        <v>41.481999999999999</v>
+        <v>40.902999999999999</v>
       </c>
       <c r="D15" s="2">
-        <v>7.6509999999999998</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E15" s="2">
-        <v>162</v>
+        <v>274</v>
       </c>
       <c r="F15" s="2">
-        <v>42049</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2">
-        <v>2139</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+        <v>35126.300000000003</v>
+      </c>
+      <c r="L15">
+        <v>1384.127</v>
+      </c>
       <c r="N15" s="2">
-        <v>885</v>
+        <v>850</v>
       </c>
       <c r="O15" s="2">
-        <v>4270.8999999999996</v>
-      </c>
-      <c r="P15" s="2"/>
+        <v>2665.5</v>
+      </c>
+      <c r="P15" s="2">
+        <v>151.80000000000001</v>
+      </c>
       <c r="Q15" s="2">
-        <v>95.557000000000002</v>
+        <v>76.257999999999996</v>
       </c>
       <c r="R15" s="2">
-        <v>1198</v>
+        <v>1089</v>
       </c>
       <c r="S15" s="2">
-        <v>14680.8</v>
+        <v>26942.7</v>
       </c>
       <c r="T15" s="2">
-        <v>210.2</v>
+        <v>91.8</v>
       </c>
       <c r="U15" s="2">
-        <v>1165</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C16" s="2">
+        <v>41</v>
+      </c>
+      <c r="D16" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>225</v>
+      </c>
+      <c r="F16" s="2">
+        <v>38166</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2544</v>
+      </c>
+      <c r="L16">
+        <v>863.57799999999997</v>
+      </c>
+      <c r="N16" s="2">
+        <v>873</v>
+      </c>
+      <c r="O16" s="2">
+        <v>3265.1</v>
+      </c>
+      <c r="P16" s="2">
+        <v>213.9</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>85.277000000000001</v>
+      </c>
+      <c r="R16" s="2">
+        <v>991</v>
+      </c>
+      <c r="S16" s="2">
+        <v>15205.4</v>
+      </c>
+      <c r="T16" s="2">
+        <v>466.7</v>
+      </c>
+      <c r="U16" s="2">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C17" s="2">
+        <v>41.481999999999999</v>
+      </c>
+      <c r="D17" s="2">
+        <v>7.6509999999999998</v>
+      </c>
+      <c r="E17" s="2">
+        <v>162</v>
+      </c>
+      <c r="F17" s="2">
+        <v>42049</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
+        <v>2139</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2">
+        <v>885</v>
+      </c>
+      <c r="O17" s="2">
+        <v>4270.8999999999996</v>
+      </c>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2">
+        <v>95.557000000000002</v>
+      </c>
+      <c r="R17" s="2">
+        <v>1198</v>
+      </c>
+      <c r="S17" s="2">
+        <v>14680.8</v>
+      </c>
+      <c r="T17" s="2">
+        <v>210.2</v>
+      </c>
+      <c r="U17" s="2">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B18" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6"/>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6">
+        <v>3497</v>
+      </c>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="4">
         <v>2017</v>
       </c>
-      <c r="U16" s="2">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4">
+        <v>24.1</v>
+      </c>
+      <c r="E19" s="4">
+        <v>467</v>
+      </c>
+      <c r="F19" s="4">
+        <v>28762</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4">
+        <v>4471</v>
+      </c>
+      <c r="O19" s="4">
+        <v>2200.6999999999998</v>
+      </c>
+      <c r="P19" s="4">
+        <v>4279.3999999999996</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>413.28899999999999</v>
+      </c>
+      <c r="R19" s="4">
+        <v>6734</v>
+      </c>
+      <c r="S19" s="4">
+        <v>17015</v>
+      </c>
+      <c r="T19" s="4">
+        <v>155.1</v>
+      </c>
+      <c r="U19" s="4">
         <v>-677</v>
       </c>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B20" s="4">
         <v>2018</v>
       </c>
-      <c r="D17" s="2">
+      <c r="C20" s="7"/>
+      <c r="D20" s="4">
         <v>24.9</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E20" s="4">
         <v>507</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F20" s="4">
         <v>31629</v>
       </c>
-      <c r="N17" s="2">
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="4">
         <v>4471</v>
       </c>
-      <c r="O17" s="2">
+      <c r="O20" s="4">
         <v>1435.5</v>
       </c>
-      <c r="P17" s="2">
+      <c r="P20" s="4">
         <v>4022.4</v>
       </c>
-      <c r="Q17" s="2">
+      <c r="Q20" s="4">
         <v>422.51900000000001</v>
       </c>
-      <c r="R17" s="2">
+      <c r="R20" s="4">
         <v>7064</v>
       </c>
-      <c r="S17" s="2">
+      <c r="S20" s="4">
         <v>20304.5</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T20" s="4">
         <v>389.4</v>
       </c>
-      <c r="U17" s="2">
+      <c r="U20" s="4">
         <v>7470</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B21" s="4">
         <v>2019</v>
       </c>
-      <c r="D18" s="2">
+      <c r="C21" s="7"/>
+      <c r="D21" s="4">
         <v>26</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E21" s="4">
         <v>743</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F21" s="4">
         <v>33185</v>
       </c>
-      <c r="N18" s="2">
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="4">
         <v>3822</v>
       </c>
-      <c r="O18" s="2">
+      <c r="O21" s="4">
         <v>1871.8</v>
       </c>
-      <c r="P18" s="2">
+      <c r="P21" s="4">
         <v>3351.1</v>
       </c>
-      <c r="Q18" s="2">
+      <c r="Q21" s="4">
         <v>484.16899999999998</v>
       </c>
-      <c r="R18" s="2">
+      <c r="R21" s="4">
         <v>9054</v>
       </c>
-      <c r="S18" s="2">
+      <c r="S21" s="4">
         <v>23432.799999999999</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T21" s="4">
         <v>749.8</v>
       </c>
-      <c r="U18" s="2">
+      <c r="U21" s="4">
         <v>10533</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B22" s="4">
         <v>2020</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C22" s="4">
         <v>88.879000000000005</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D22" s="4">
         <v>26.6</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E22" s="4">
         <v>5378</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F22" s="4">
         <v>34049</v>
       </c>
-      <c r="N19" s="2">
+      <c r="G22" s="7"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="4">
         <v>3562</v>
       </c>
-      <c r="O19" s="2">
+      <c r="O22" s="4">
         <v>1845</v>
       </c>
-      <c r="P19" s="2">
+      <c r="P22" s="4">
         <v>637.29999999999995</v>
       </c>
-      <c r="Q19" s="2">
+      <c r="Q22" s="4">
         <v>526.50900000000001</v>
       </c>
-      <c r="R19" s="2">
+      <c r="R22" s="4">
         <v>9241</v>
       </c>
-      <c r="S19" s="2">
+      <c r="S22" s="4">
         <v>26593</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T22" s="4">
         <v>753.2</v>
       </c>
-      <c r="U19" s="2">
+      <c r="U22" s="4">
         <v>7130</v>
       </c>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B23" s="4">
         <v>2021</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C23" s="4">
         <v>81.863</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D23" s="4">
         <v>28.3</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E23" s="4">
         <v>1017</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F23" s="4">
         <v>38808</v>
       </c>
-      <c r="L20">
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7">
         <v>15703.486000000001</v>
       </c>
-      <c r="N20" s="2">
+      <c r="M23" s="7"/>
+      <c r="N23" s="4">
         <v>3561</v>
       </c>
-      <c r="O20" s="2">
+      <c r="O23" s="4">
         <v>2466.6999999999998</v>
       </c>
-      <c r="P20" s="2">
+      <c r="P23" s="4">
         <v>289.2</v>
       </c>
-      <c r="Q20" s="2">
+      <c r="Q23" s="4">
         <v>523.16399999999999</v>
       </c>
-      <c r="R20" s="2">
+      <c r="R23" s="4">
         <v>8415</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S23" s="4">
         <v>36829.599999999999</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T23" s="4">
         <v>1014.6</v>
       </c>
-      <c r="U20" s="2">
+      <c r="U23" s="4">
         <v>1556</v>
       </c>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B24" s="4">
         <v>2022</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C24" s="4">
         <v>81.863</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D24" s="4">
         <v>29</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E24" s="4">
         <v>929</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F24" s="4">
         <v>42361</v>
       </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2">
+      <c r="G24" s="4"/>
+      <c r="H24" s="4">
         <v>8508</v>
       </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2">
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4">
         <v>26447.994999999999</v>
       </c>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2">
+      <c r="M24" s="4"/>
+      <c r="N24" s="4">
         <v>3334</v>
       </c>
-      <c r="O21" s="2">
+      <c r="O24" s="4">
         <v>3321.5</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P24" s="4">
         <v>150.80000000000001</v>
       </c>
-      <c r="Q21" s="2">
+      <c r="Q24" s="4">
         <v>532.51300000000003</v>
       </c>
-      <c r="R21" s="2">
+      <c r="R24" s="4">
         <v>5456</v>
       </c>
-      <c r="S21" s="2">
+      <c r="S24" s="4">
         <v>41571.199999999997</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T24" s="4">
         <v>2116</v>
       </c>
-      <c r="U21" s="2">
+      <c r="U24" s="4">
         <v>704</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B25" s="4">
         <v>2023</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C25" s="4">
         <v>82.691999999999993</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D25" s="4">
         <v>30.728999999999999</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E25" s="4">
         <v>643</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F25" s="4">
         <v>49270</v>
       </c>
-      <c r="H22" s="2">
+      <c r="G25" s="7"/>
+      <c r="H25" s="4">
         <v>8508</v>
       </c>
-      <c r="N22" s="2">
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="4">
         <v>3373</v>
       </c>
-      <c r="O22" s="2">
+      <c r="O25" s="4">
         <v>5465.4</v>
       </c>
-      <c r="Q22" s="2">
+      <c r="P25" s="7"/>
+      <c r="Q25" s="4">
         <v>592.06500000000005</v>
       </c>
-      <c r="R22" s="2">
+      <c r="R25" s="4">
         <v>7363</v>
       </c>
-      <c r="S22" s="2">
+      <c r="S25" s="4">
         <v>49034.2</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T25" s="4">
         <v>3455.4180000000001</v>
       </c>
-      <c r="U22" s="2">
+      <c r="U25" s="4">
         <v>4899</v>
       </c>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B26" s="6">
+        <v>2016</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6">
+        <v>-235</v>
+      </c>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="4">
         <v>2017</v>
       </c>
-      <c r="U23" s="2">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4">
+        <v>16.2</v>
+      </c>
+      <c r="E27" s="4">
+        <v>194</v>
+      </c>
+      <c r="F27" s="4">
+        <v>30578</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4">
+        <v>3047</v>
+      </c>
+      <c r="O27" s="4">
+        <v>1638.7</v>
+      </c>
+      <c r="P27" s="4">
+        <v>401.5</v>
+      </c>
+      <c r="Q27" s="4">
+        <v>82.164000000000001</v>
+      </c>
+      <c r="R27" s="4">
+        <v>983</v>
+      </c>
+      <c r="S27" s="4">
+        <v>10482.700000000001</v>
+      </c>
+      <c r="T27" s="4">
+        <v>774.9</v>
+      </c>
+      <c r="U27" s="4">
         <v>2138</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="2">
-        <v>2018</v>
-      </c>
-      <c r="D24" s="2">
-        <v>17</v>
-      </c>
-      <c r="E24" s="2">
-        <v>196</v>
-      </c>
-      <c r="F24" s="2">
-        <v>33853</v>
-      </c>
-      <c r="N24" s="2">
-        <v>3047</v>
-      </c>
-      <c r="O24" s="2">
-        <v>1997.1</v>
-      </c>
-      <c r="P24" s="2">
-        <v>174.9</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>111.617</v>
-      </c>
-      <c r="R24" s="2">
-        <v>1622</v>
-      </c>
-      <c r="S24" s="2">
-        <v>13072.3</v>
-      </c>
-      <c r="T24" s="2">
-        <v>753.8</v>
-      </c>
-      <c r="U24" s="2">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2019</v>
-      </c>
-      <c r="D25" s="2">
-        <v>17.2</v>
-      </c>
-      <c r="E25" s="2">
-        <v>266</v>
-      </c>
-      <c r="F25" s="2">
-        <v>36573</v>
-      </c>
-      <c r="N25" s="2">
-        <v>2717</v>
-      </c>
-      <c r="O25" s="2">
-        <v>2218.6999999999998</v>
-      </c>
-      <c r="P25" s="2">
-        <v>200.3</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>85.382999999999996</v>
-      </c>
-      <c r="R25" s="2">
-        <v>915</v>
-      </c>
-      <c r="S25" s="2">
-        <v>14798.4</v>
-      </c>
-      <c r="T25" s="2">
-        <v>878.2</v>
-      </c>
-      <c r="U25" s="2">
-        <v>-553</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2">
-        <v>2020</v>
-      </c>
-      <c r="C26" s="2">
-        <v>76.783000000000001</v>
-      </c>
-      <c r="D26" s="2">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="E26" s="2">
-        <v>894</v>
-      </c>
-      <c r="F26" s="2">
-        <v>37974</v>
-      </c>
-      <c r="N26" s="2">
-        <v>2586</v>
-      </c>
-      <c r="O26" s="2">
-        <v>1326.7</v>
-      </c>
-      <c r="P26" s="2">
-        <v>1094.7</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>74.545000000000002</v>
-      </c>
-      <c r="R26" s="2">
-        <v>416</v>
-      </c>
-      <c r="S26" s="2">
-        <v>17282</v>
-      </c>
-      <c r="T26" s="2">
-        <v>1027.8</v>
-      </c>
-      <c r="U26" s="2">
-        <v>-1278</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="2">
-        <v>2021</v>
-      </c>
-      <c r="C27" s="2">
-        <v>80.203999999999994</v>
-      </c>
-      <c r="D27" s="2">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E27" s="2">
-        <v>262</v>
-      </c>
-      <c r="F27" s="2">
-        <v>42904</v>
-      </c>
-      <c r="L27">
-        <v>10326.647999999999</v>
-      </c>
-      <c r="N27" s="2">
-        <v>2565</v>
-      </c>
-      <c r="O27" s="2">
-        <v>1318.4</v>
-      </c>
-      <c r="P27" s="2">
-        <v>4092.5</v>
-      </c>
-      <c r="Q27" s="2">
-        <v>101.312</v>
-      </c>
-      <c r="R27" s="2">
-        <v>552</v>
-      </c>
-      <c r="S27" s="2">
-        <v>24283.1</v>
-      </c>
-      <c r="T27" s="2">
-        <v>992.7</v>
-      </c>
-      <c r="U27" s="2">
-        <v>-258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B28" s="2">
-        <v>2022</v>
-      </c>
-      <c r="C28" s="2">
-        <v>80.203999999999994</v>
+        <v>2018</v>
       </c>
       <c r="D28" s="2">
-        <v>18.2</v>
+        <v>17</v>
       </c>
       <c r="E28" s="2">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="F28" s="2">
-        <v>48384</v>
-      </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2">
-        <v>5843</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2">
-        <v>7713.7349999999997</v>
-      </c>
-      <c r="M28" s="2"/>
+        <v>33853</v>
+      </c>
       <c r="N28" s="2">
-        <v>2489</v>
+        <v>3047</v>
       </c>
       <c r="O28" s="2">
-        <v>2937.3</v>
+        <v>1997.1</v>
       </c>
       <c r="P28" s="2">
-        <v>3009</v>
+        <v>174.9</v>
       </c>
       <c r="Q28" s="2">
-        <v>188.37</v>
+        <v>111.617</v>
       </c>
       <c r="R28" s="2">
-        <v>970</v>
+        <v>1622</v>
       </c>
       <c r="S28" s="2">
-        <v>27967.1</v>
+        <v>13072.3</v>
       </c>
       <c r="T28" s="2">
-        <v>631.20000000000005</v>
+        <v>753.8</v>
       </c>
       <c r="U28" s="2">
-        <v>-366</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="2">
+        <v>2019</v>
+      </c>
+      <c r="D29" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="E29" s="2">
+        <v>266</v>
+      </c>
+      <c r="F29" s="2">
+        <v>36573</v>
+      </c>
+      <c r="N29" s="2">
+        <v>2717</v>
+      </c>
+      <c r="O29" s="2">
+        <v>2218.6999999999998</v>
+      </c>
+      <c r="P29" s="2">
+        <v>200.3</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>85.382999999999996</v>
+      </c>
+      <c r="R29" s="2">
+        <v>915</v>
+      </c>
+      <c r="S29" s="2">
+        <v>14798.4</v>
+      </c>
+      <c r="T29" s="2">
+        <v>878.2</v>
+      </c>
+      <c r="U29" s="2">
+        <v>-553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C30" s="2">
+        <v>76.783000000000001</v>
+      </c>
+      <c r="D30" s="2">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="E30" s="2">
+        <v>894</v>
+      </c>
+      <c r="F30" s="2">
+        <v>37974</v>
+      </c>
+      <c r="N30" s="2">
+        <v>2586</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1326.7</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1094.7</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>74.545000000000002</v>
+      </c>
+      <c r="R30" s="2">
+        <v>416</v>
+      </c>
+      <c r="S30" s="2">
+        <v>17282</v>
+      </c>
+      <c r="T30" s="2">
+        <v>1027.8</v>
+      </c>
+      <c r="U30" s="2">
+        <v>-1278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C31" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D31" s="2">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E31" s="2">
+        <v>262</v>
+      </c>
+      <c r="F31" s="2">
+        <v>42904</v>
+      </c>
+      <c r="L31">
+        <v>10326.647999999999</v>
+      </c>
+      <c r="N31" s="2">
+        <v>2565</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1318.4</v>
+      </c>
+      <c r="P31" s="2">
+        <v>4092.5</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>101.312</v>
+      </c>
+      <c r="R31" s="2">
+        <v>552</v>
+      </c>
+      <c r="S31" s="2">
+        <v>24283.1</v>
+      </c>
+      <c r="T31" s="2">
+        <v>992.7</v>
+      </c>
+      <c r="U31" s="2">
+        <v>-258</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C32" s="2">
+        <v>80.203999999999994</v>
+      </c>
+      <c r="D32" s="2">
+        <v>18.2</v>
+      </c>
+      <c r="E32" s="2">
+        <v>212</v>
+      </c>
+      <c r="F32" s="2">
+        <v>48384</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2">
+        <v>5843</v>
+      </c>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2">
+        <v>7713.7349999999997</v>
+      </c>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2">
+        <v>2489</v>
+      </c>
+      <c r="O32" s="2">
+        <v>2937.3</v>
+      </c>
+      <c r="P32" s="2">
+        <v>3009</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>188.37</v>
+      </c>
+      <c r="R32" s="2">
+        <v>970</v>
+      </c>
+      <c r="S32" s="2">
+        <v>27967.1</v>
+      </c>
+      <c r="T32" s="2">
+        <v>631.20000000000005</v>
+      </c>
+      <c r="U32" s="2">
+        <v>-366</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="2">
         <v>2023</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C33" s="2">
         <v>80.296000000000006</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D33" s="2">
         <v>19.093</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E33" s="2">
         <v>96</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F33" s="2">
         <v>56182</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H33" s="2">
         <v>5703</v>
       </c>
-      <c r="N29" s="2">
+      <c r="N33" s="2">
         <v>2396</v>
       </c>
-      <c r="O29" s="2">
+      <c r="O33" s="2">
         <v>3456.8</v>
       </c>
-      <c r="P29" s="2">
+      <c r="P33" s="2">
         <v>12221.3</v>
       </c>
-      <c r="Q29" s="2">
+      <c r="Q33" s="2">
         <v>114.619</v>
       </c>
-      <c r="R29" s="2">
+      <c r="R33" s="2">
         <v>646</v>
       </c>
-      <c r="S29" s="2">
+      <c r="S33" s="2">
         <v>32472.3</v>
       </c>
-      <c r="T29" s="2">
+      <c r="T33" s="2">
         <v>1040.3309999999999</v>
       </c>
-      <c r="U29" s="2">
+      <c r="U33" s="2">
         <v>407</v>
       </c>
     </row>

</xml_diff>